<commit_message>
EPBDS-8167 fix casting NullOpenClass to Primitive Type. Primitive default value must be returned
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-2619_IntBoolExp.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-2619_IntBoolExp.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2859234E-E880-42C0-A335-954CD4F36A20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alias" sheetId="3" r:id="rId1"/>
@@ -14,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Tatsiana Ulyanava</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -45,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0">
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -198,7 +204,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -356,14 +362,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -374,9 +372,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -384,14 +390,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -429,9 +438,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -464,9 +473,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,9 +525,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -674,11 +717,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="L24:M24"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,18 +736,18 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="F4" s="24" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="F4" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="23" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -721,7 +764,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="20"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
@@ -739,38 +782,38 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="5">
         <v>40722</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="19" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="6">
         <v>1</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="19" t="s">
         <v>24</v>
       </c>
       <c r="G8" s="6">
         <v>1</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="19" t="s">
         <v>24</v>
       </c>
     </row>
@@ -778,18 +821,18 @@
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="F9" s="23">
+      <c r="D9" s="23"/>
+      <c r="F9" s="19">
         <v>12</v>
       </c>
       <c r="G9" s="6">
         <v>2</v>
       </c>
       <c r="H9" s="9"/>
-      <c r="I9" s="23">
+      <c r="I9" s="19">
         <v>12</v>
       </c>
     </row>
@@ -797,18 +840,18 @@
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="F10" s="23">
+      <c r="D10" s="23"/>
+      <c r="F10" s="19">
         <v>13</v>
       </c>
       <c r="G10" s="6">
         <v>3</v>
       </c>
       <c r="H10" s="9"/>
-      <c r="I10" s="23">
+      <c r="I10" s="19">
         <v>13</v>
       </c>
     </row>
@@ -816,15 +859,17 @@
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="F11" s="23" t="s">
+      <c r="D11" s="23"/>
+      <c r="F11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="I11" s="23" t="s">
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="19" t="s">
         <v>25</v>
       </c>
     </row>
@@ -832,17 +877,17 @@
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="F12" s="23" t="s">
+      <c r="D12" s="23"/>
+      <c r="F12" s="19" t="s">
         <v>20</v>
       </c>
       <c r="G12" s="6">
         <v>1</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="19" t="s">
         <v>20</v>
       </c>
     </row>
@@ -850,47 +895,47 @@
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="23">
         <v>1</v>
       </c>
-      <c r="D13" s="20"/>
+      <c r="D13" s="23"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="23">
         <v>2</v>
       </c>
-      <c r="D14" s="20"/>
+      <c r="D14" s="23"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="23">
         <v>3</v>
       </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="23"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="23">
         <v>4</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="23"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="23" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -901,7 +946,7 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="20"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="8" t="s">
         <v>14</v>
       </c>
@@ -910,7 +955,7 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="20"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="17" t="s">
         <v>9</v>
       </c>
@@ -919,7 +964,7 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="16" t="s">
         <v>7</v>
       </c>
@@ -931,33 +976,33 @@
       <c r="B25" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="20"/>
+      <c r="D25" s="23"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="F26" s="24" t="s">
+      <c r="D26" s="23"/>
+      <c r="F26" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="25"/>
-      <c r="H26" s="26"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="22"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="20"/>
+      <c r="D27" s="23"/>
       <c r="F27" s="6" t="s">
         <v>12</v>
       </c>
@@ -972,10 +1017,10 @@
       <c r="B28" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="20"/>
+      <c r="D28" s="23"/>
       <c r="F28" s="6" t="s">
         <v>17</v>
       </c>
@@ -990,11 +1035,11 @@
       <c r="B29" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="23">
         <v>1</v>
       </c>
-      <c r="D29" s="20"/>
-      <c r="F29" s="23" t="s">
+      <c r="D29" s="23"/>
+      <c r="F29" s="19" t="s">
         <v>31</v>
       </c>
       <c r="G29" s="6">
@@ -1008,11 +1053,11 @@
       <c r="B30" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="23">
         <v>2</v>
       </c>
-      <c r="D30" s="20"/>
-      <c r="F30" s="23" t="s">
+      <c r="D30" s="23"/>
+      <c r="F30" s="19" t="s">
         <v>32</v>
       </c>
       <c r="G30" s="6">
@@ -1023,14 +1068,20 @@
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F31" s="23"/>
-      <c r="G31" s="6"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="6">
+        <v>0</v>
+      </c>
       <c r="H31" s="6" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="F26:H26"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B21:B24"/>
@@ -1047,10 +1098,6 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>